<commit_message>
testing and new data
</commit_message>
<xml_diff>
--- a/data/TWP emission data_IDIADA_v01.xlsx
+++ b/data/TWP emission data_IDIADA_v01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rivmnl.sharepoint.com/sites/LEON-Tyres/Gedeelde documenten/WP3 Microplastics/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1265" documentId="8_{0C357616-BE86-4C54-B640-5799EF490498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{557D1D02-665C-4295-8E46-505AF27AB255}"/>
+  <xr:revisionPtr revIDLastSave="1471" documentId="8_{0C357616-BE86-4C54-B640-5799EF490498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86DAB85C-BF67-46AB-B7AF-7C568F21FFD9}"/>
   <bookViews>
-    <workbookView xWindow="13410" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1B08EC6D-E4F6-452D-BA0B-C8BBC214CF8F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1B08EC6D-E4F6-452D-BA0B-C8BBC214CF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -20,9 +20,11 @@
     <sheet name="Vehicle data" sheetId="3" r:id="rId5"/>
     <sheet name="Tyre_data" sheetId="4" r:id="rId6"/>
     <sheet name="Abrasion" sheetId="11" r:id="rId7"/>
-    <sheet name="Constants" sheetId="5" r:id="rId8"/>
-    <sheet name="Label fuel efficiency class" sheetId="6" state="hidden" r:id="rId9"/>
-    <sheet name="Label wet grip class" sheetId="7" state="hidden" r:id="rId10"/>
+    <sheet name="Tyre_ADAC" sheetId="13" r:id="rId8"/>
+    <sheet name="Abrasion_ADAC" sheetId="12" r:id="rId9"/>
+    <sheet name="Constants" sheetId="5" r:id="rId10"/>
+    <sheet name="Label fuel efficiency class" sheetId="6" state="hidden" r:id="rId11"/>
+    <sheet name="Label wet grip class" sheetId="7" state="hidden" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -76,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Joris Quik:</t>
         </r>
@@ -85,7 +87,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Coincides with the the Abrasion test data, where the T1-T5 stand for repeats of the same test</t>
@@ -143,6 +145,7 @@
   <authors>
     <author>Joris Quik</author>
     <author>tc={E549596F-1E58-4DED-8B53-CF6FA51991B1}</author>
+    <author>tc={DDA64BFA-D28D-4B7C-B35C-90CB1298EE69}</author>
   </authors>
   <commentList>
     <comment ref="D1" authorId="0" shapeId="0" xr:uid="{F3C22D7F-5376-4643-80A9-2D37A3FB0FEA}">
@@ -153,7 +156,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Joris Quik:</t>
         </r>
@@ -162,7 +165,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Mass in the AbrasionTest</t>
@@ -189,7 +192,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Joris Quik:</t>
         </r>
@@ -198,11 +201,111 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 High temperature added just for convencience, but no difference in calculations</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="2" shapeId="0" xr:uid="{DDA64BFA-D28D-4B7C-B35C-90CB1298EE69}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+[Tasks]
+There is a task anchored to this comment that cannot be viewed in your client.
+Comment:
+    @Joris Meesters , ADAC heeft een VW polo gebruikt toch? Zou je voor interpreteren van de ADAC gegevens de waarden hiervoor willen invullen? Ik kon ze niet meer vinden.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={74A80BAF-D6C7-46BC-B829-ED1B8A239F99}</author>
+    <author>tc={0D79CBC1-2634-45C8-9083-88EF78337D3C}</author>
+    <author>tc={6C100F98-F6FB-45F9-87E2-D6113A56C424}</author>
+    <author>tc={7C540CA7-1742-41AA-8C18-2D835D3B4F82}</author>
+  </authors>
+  <commentList>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{74A80BAF-D6C7-46BC-B829-ED1B8A239F99}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    TWO labels *AB or BB</t>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="1" shapeId="0" xr:uid="{0D79CBC1-2634-45C8-9083-88EF78337D3C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Niet in EPREL data base (label van ADAC site) https://www.adac.de/rund-ums-fahrzeug/ausstattung-technik-zubehoer/reifen/reifentest/sommerreifen/205-55-r16/king-meiler-sport-1-id-4476/</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="2" shapeId="0" xr:uid="{6C100F98-F6FB-45F9-87E2-D6113A56C424}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Premitra 5 niet terug te vinden, gebruik label van HP5 model</t>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="3" shapeId="0" xr:uid="{7C540CA7-1742-41AA-8C18-2D835D3B4F82}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Many different ones with raning (also other brands, different on martket dates). Used 40605 label</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={5C32FB0E-B292-4226-A4D7-0FC189658EDC}</author>
+    <author>tc={F847441E-647B-4A01-89C5-91E38E7644E4}</author>
+    <author>tc={F0920C63-E50A-4591-A7F2-970D431E17A9}</author>
+    <author>tc={2567C819-AF5D-4925-828A-E46A4F184DA4}</author>
+  </authors>
+  <commentList>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{5C32FB0E-B292-4226-A4D7-0FC189658EDC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    TWO labels *AB or BB</t>
+      </text>
+    </comment>
+    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{F847441E-647B-4A01-89C5-91E38E7644E4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Niet in EPREL data base (label van ADAC site) https://www.adac.de/rund-ums-fahrzeug/ausstattung-technik-zubehoer/reifen/reifentest/sommerreifen/205-55-r16/king-meiler-sport-1-id-4476/</t>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="2" shapeId="0" xr:uid="{F0920C63-E50A-4591-A7F2-970D431E17A9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Premitra 5 niet terug te vinden, gebruik label van HP5 model</t>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="3" shapeId="0" xr:uid="{2567C819-AF5D-4925-828A-E46A4F184DA4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Many different ones with raning (also other brands, different on martket dates). Used 40605 label</t>
       </text>
     </comment>
   </commentList>
@@ -210,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1059" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="400">
   <si>
     <t>This is a spreadsheet collecting all the data needed to apply the tyre friction abrasion model.</t>
   </si>
@@ -1212,6 +1315,204 @@
   </si>
   <si>
     <t>Label_wet_grip_class</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Tyre name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADAC wear g per 1000 km </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goodyear Efficient Grip Performance 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fulda Ecocontrol HP2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petlas Imperium PT515 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kumho Ecsta HS51 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apollo Alnac 4G </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BF Goodrich Advantage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bridgestone Turanza T005 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">King Meiler Sport 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semperit Speed-Life 3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continental Premium Contact 6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxxis Premitra 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hankook Ventus Prime 3 K125 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uniroyal Rainsport 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pirelli Cinturato P7 C2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nokian Wetproof </t>
+  </si>
+  <si>
+    <t>Abrasion_ADAC</t>
+  </si>
+  <si>
+    <t>ADAC data for Summer tyres 205/55 R16 (2021) (Data need: tyre identifyer *EPREL, now choosing SL if unclear.)</t>
+  </si>
+  <si>
+    <t>ADAC_T_A1</t>
+  </si>
+  <si>
+    <t>ADAC_T_A2</t>
+  </si>
+  <si>
+    <t>ADAC_T_A3</t>
+  </si>
+  <si>
+    <t>ADAC_T_A4</t>
+  </si>
+  <si>
+    <t>ADAC_T_A5</t>
+  </si>
+  <si>
+    <t>ADAC_T_A6</t>
+  </si>
+  <si>
+    <t>ADAC_T_A7</t>
+  </si>
+  <si>
+    <t>ADAC_T_A8</t>
+  </si>
+  <si>
+    <t>ADAC_T_A9</t>
+  </si>
+  <si>
+    <t>ADAC_T_A10</t>
+  </si>
+  <si>
+    <t>ADAC_T_A11</t>
+  </si>
+  <si>
+    <t>ADAC_T_A12</t>
+  </si>
+  <si>
+    <t>ADAC_T_A13</t>
+  </si>
+  <si>
+    <t>ADAC_T_A14</t>
+  </si>
+  <si>
+    <t>ADAC_T_A15</t>
+  </si>
+  <si>
+    <t>Fulda</t>
+  </si>
+  <si>
+    <t>Petlas</t>
+  </si>
+  <si>
+    <t>Kumho</t>
+  </si>
+  <si>
+    <t>Apollo</t>
+  </si>
+  <si>
+    <t>Bridgestone</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>Semperit</t>
+  </si>
+  <si>
+    <t>Continental</t>
+  </si>
+  <si>
+    <t>Maxxis</t>
+  </si>
+  <si>
+    <t>Hankook</t>
+  </si>
+  <si>
+    <t>Uniroyal</t>
+  </si>
+  <si>
+    <t>Nokian</t>
+  </si>
+  <si>
+    <t>BFGoodrich</t>
+  </si>
+  <si>
+    <t>Motorway straight</t>
+  </si>
+  <si>
+    <t>Motorway bends</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>MMoWStr1</t>
+  </si>
+  <si>
+    <t>MMoWStr2</t>
+  </si>
+  <si>
+    <t>MMoWStr3</t>
+  </si>
+  <si>
+    <t>MMoWStr4</t>
+  </si>
+  <si>
+    <t>Golf 7 Facelift</t>
+  </si>
+  <si>
+    <t>ADAC</t>
+  </si>
+  <si>
+    <t>SIML1</t>
+  </si>
+  <si>
+    <t>SIML2</t>
+  </si>
+  <si>
+    <t>East BendSIML</t>
+  </si>
+  <si>
+    <t>North StraightSIML</t>
+  </si>
+  <si>
+    <t>Oval Outer LaneSIML</t>
+  </si>
+  <si>
+    <t>MotorwaySIML</t>
+  </si>
+  <si>
+    <t>Motorway_SIML</t>
+  </si>
+  <si>
+    <t>Motorway_SIML_straight</t>
+  </si>
+  <si>
+    <t>Motorway_SIML_bend</t>
   </si>
 </sst>
 </file>
@@ -1260,17 +1561,17 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1310,6 +1611,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1523,7 +1836,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1578,6 +1891,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1614,6 +1929,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda 2" xfId="1" xr:uid="{CFCD8E07-CE35-4F1F-B23D-4B3C1756CB7C}"/>
@@ -1633,8 +1949,42 @@
 </styleSheet>
 </file>
 
+<file path=xl/documenttasks/documenttask1.xml><?xml version="1.0" encoding="utf-8"?>
+<Tasks xmlns="http://schemas.microsoft.com/office/tasks/2019/documenttasks">
+  <Task id="{5D13ECFB-BB48-4CF3-90B8-66FDCD19F7E3}">
+    <Anchor>
+      <Comment id="{DDA64BFA-D28D-4B7C-B35C-90CB1298EE69}"/>
+    </Anchor>
+    <History>
+      <Event time="2024-04-22T08:39:46.83" id="{B8EBB1D8-2112-408F-8705-989D570FA7AD}">
+        <Attribution userId="S::joris.quik@rivm.nl::d9be75de-0916-4104-a6e9-f041d63f8124" userName="Joris Quik" userProvider="AD"/>
+        <Anchor>
+          <Comment id="{DDA64BFA-D28D-4B7C-B35C-90CB1298EE69}"/>
+        </Anchor>
+        <Create/>
+      </Event>
+      <Event time="2024-04-22T08:39:46.83" id="{567A07E4-2D1F-4EB0-8D5C-999A9F96D5E1}">
+        <Attribution userId="S::joris.quik@rivm.nl::d9be75de-0916-4104-a6e9-f041d63f8124" userName="Joris Quik" userProvider="AD"/>
+        <Anchor>
+          <Comment id="{DDA64BFA-D28D-4B7C-B35C-90CB1298EE69}"/>
+        </Anchor>
+        <Assign userId="S::joris.meesters@rivm.nl::7355ad4c-5157-4909-b794-36d8e163cb31" userName="Joris Meesters" userProvider="AD"/>
+      </Event>
+      <Event time="2024-04-22T08:39:46.83" id="{179D4FD1-2CE9-4616-8FB8-91B8D38A524B}">
+        <Attribution userId="S::joris.quik@rivm.nl::d9be75de-0916-4104-a6e9-f041d63f8124" userName="Joris Quik" userProvider="AD"/>
+        <Anchor>
+          <Comment id="{DDA64BFA-D28D-4B7C-B35C-90CB1298EE69}"/>
+        </Anchor>
+        <SetTitle title="@Joris Meesters , ADAC heeft een VW polo gebruikt toch? Zou je voor interpreteren van de ADAC gegevens de waarden hiervoor willen invullen? Ik kon ze niet meer vinden."/>
+      </Event>
+    </History>
+  </Task>
+</Tasks>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Joris Quik" id="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" userId="Joris Quik" providerId="None"/>
   <person displayName="Joris Meesters" id="{1C83AC79-71CA-44C2-9747-7E48DA48E1AF}" userId="joris.meesters@rivm.nl" providerId="PeoplePicker"/>
   <person displayName="Joris Quik" id="{F1BB3989-B25A-49D2-B8F1-B653F64BFBB8}" userId="S::joris.quik@rivm.nl::d9be75de-0916-4104-a6e9-f041d63f8124" providerId="AD"/>
   <person displayName="Joris Meesters" id="{A5D964E5-E453-44CF-A675-06CD4C5F042C}" userId="S::joris.meesters@rivm.nl::7355ad4c-5157-4909-b794-36d8e163cb31" providerId="AD"/>
@@ -1990,15 +2340,55 @@
   <threadedComment ref="D3" dT="2024-04-18T10:26:06.17" personId="{A5D964E5-E453-44CF-A675-06CD4C5F042C}" id="{02A810B8-3B32-4E3D-93F0-F151DB15B371}" parentId="{E549596F-1E58-4DED-8B53-CF6FA51991B1}">
     <text>correct</text>
   </threadedComment>
+  <threadedComment ref="A5" dT="2024-04-22T08:39:46.83" personId="{F1BB3989-B25A-49D2-B8F1-B653F64BFBB8}" id="{DDA64BFA-D28D-4B7C-B35C-90CB1298EE69}">
+    <text>@Joris Meesters , ADAC heeft een VW polo gebruikt toch? Zou je voor interpreteren van de ADAC gegevens de waarden hiervoor willen invullen? Ik kon ze niet meer vinden.</text>
+    <mentions>
+      <mention mentionpersonId="{1C83AC79-71CA-44C2-9747-7E48DA48E1AF}" mentionId="{2B95CB15-D40C-4545-9AA5-30B7798E978B}" startIndex="0" length="15"/>
+    </mentions>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B8" dT="2023-06-16T12:48:08.77" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{74A80BAF-D6C7-46BC-B829-ED1B8A239F99}">
+    <text>TWO labels *AB or BB</text>
+  </threadedComment>
+  <threadedComment ref="B9" dT="2023-06-16T12:51:46.08" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{0D79CBC1-2634-45C8-9083-88EF78337D3C}">
+    <text>Niet in EPREL data base (label van ADAC site) https://www.adac.de/rund-ums-fahrzeug/ausstattung-technik-zubehoer/reifen/reifentest/sommerreifen/205-55-r16/king-meiler-sport-1-id-4476/</text>
+  </threadedComment>
+  <threadedComment ref="B12" dT="2023-06-16T12:57:18.32" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{6C100F98-F6FB-45F9-87E2-D6113A56C424}">
+    <text>Premitra 5 niet terug te vinden, gebruik label van HP5 model</text>
+  </threadedComment>
+  <threadedComment ref="B15" dT="2023-06-16T13:03:23.81" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{7C540CA7-1742-41AA-8C18-2D835D3B4F82}">
+    <text>Many different ones with raning (also other brands, different on martket dates). Used 40605 label</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment5.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A8" dT="2023-06-16T12:48:08.77" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{5C32FB0E-B292-4226-A4D7-0FC189658EDC}">
+    <text>TWO labels *AB or BB</text>
+  </threadedComment>
+  <threadedComment ref="A9" dT="2023-06-16T12:51:46.08" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{F847441E-647B-4A01-89C5-91E38E7644E4}">
+    <text>Niet in EPREL data base (label van ADAC site) https://www.adac.de/rund-ums-fahrzeug/ausstattung-technik-zubehoer/reifen/reifentest/sommerreifen/205-55-r16/king-meiler-sport-1-id-4476/</text>
+  </threadedComment>
+  <threadedComment ref="A12" dT="2023-06-16T12:57:18.32" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{F0920C63-E50A-4591-A7F2-970D431E17A9}">
+    <text>Premitra 5 niet terug te vinden, gebruik label van HP5 model</text>
+  </threadedComment>
+  <threadedComment ref="A15" dT="2023-06-16T13:03:23.81" personId="{E04D0CC9-932F-4577-9D81-3BA1E2CD2B36}" id="{2567C819-AF5D-4925-828A-E46A4F184DA4}">
+    <text>Many different ones with raning (also other brands, different on martket dates). Used 40605 label</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96033017-F400-401C-8E8A-3EF7780FA468}">
-  <dimension ref="A2:B11"/>
+  <dimension ref="A2:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2074,6 +2464,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>353</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2081,6 +2479,657 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E0172C-DF0F-4DBA-8FF0-B64EC2D7369B}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" t="s">
+        <v>301</v>
+      </c>
+      <c r="C2">
+        <v>9.81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C3">
+        <v>0.85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>306</v>
+      </c>
+      <c r="B4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4">
+        <v>0.13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5">
+        <v>0.15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C6">
+        <v>1.2050000000000001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7">
+        <v>1.07</v>
+      </c>
+      <c r="D7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B8" t="s">
+        <v>316</v>
+      </c>
+      <c r="C8">
+        <v>1.47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>319</v>
+      </c>
+      <c r="B10" t="s">
+        <v>318</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>320</v>
+      </c>
+      <c r="B11" t="s">
+        <v>318</v>
+      </c>
+      <c r="C11">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>321</v>
+      </c>
+      <c r="B12" t="s">
+        <v>318</v>
+      </c>
+      <c r="C12">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>322</v>
+      </c>
+      <c r="B13" t="s">
+        <v>323</v>
+      </c>
+      <c r="C13">
+        <v>0.68</v>
+      </c>
+      <c r="D13" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F501E61A-82C5-43C3-BC60-CB8CE2E4C1FF}">
+  <dimension ref="A1:D31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" t="s">
+        <v>328</v>
+      </c>
+      <c r="C2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2">
+        <v>5.8500000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B4" t="s">
+        <v>328</v>
+      </c>
+      <c r="C4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B5" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>229</v>
+      </c>
+      <c r="B6" t="s">
+        <v>328</v>
+      </c>
+      <c r="C6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D6">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C7" t="s">
+        <v>242</v>
+      </c>
+      <c r="D7">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B8" t="s">
+        <v>330</v>
+      </c>
+      <c r="C8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9" t="s">
+        <v>247</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B10" t="s">
+        <v>330</v>
+      </c>
+      <c r="C10" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B11" t="s">
+        <v>330</v>
+      </c>
+      <c r="C11" t="s">
+        <v>329</v>
+      </c>
+      <c r="D11">
+        <v>11.66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>331</v>
+      </c>
+      <c r="B12" t="s">
+        <v>328</v>
+      </c>
+      <c r="C12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D12">
+        <v>4.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>331</v>
+      </c>
+      <c r="B13" t="s">
+        <v>328</v>
+      </c>
+      <c r="C13" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>331</v>
+      </c>
+      <c r="B14" t="s">
+        <v>328</v>
+      </c>
+      <c r="C14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>331</v>
+      </c>
+      <c r="B15" t="s">
+        <v>328</v>
+      </c>
+      <c r="C15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D15">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>331</v>
+      </c>
+      <c r="B16" t="s">
+        <v>328</v>
+      </c>
+      <c r="C16" t="s">
+        <v>329</v>
+      </c>
+      <c r="D16">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>331</v>
+      </c>
+      <c r="B17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C17" t="s">
+        <v>242</v>
+      </c>
+      <c r="D17">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>331</v>
+      </c>
+      <c r="B18" t="s">
+        <v>330</v>
+      </c>
+      <c r="C18" t="s">
+        <v>248</v>
+      </c>
+      <c r="D18">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>331</v>
+      </c>
+      <c r="B19" t="s">
+        <v>330</v>
+      </c>
+      <c r="C19" t="s">
+        <v>247</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>331</v>
+      </c>
+      <c r="B20" t="s">
+        <v>330</v>
+      </c>
+      <c r="C20" t="s">
+        <v>241</v>
+      </c>
+      <c r="D20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>331</v>
+      </c>
+      <c r="B21" t="s">
+        <v>330</v>
+      </c>
+      <c r="C21" t="s">
+        <v>329</v>
+      </c>
+      <c r="D21">
+        <v>10.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>332</v>
+      </c>
+      <c r="B22" t="s">
+        <v>328</v>
+      </c>
+      <c r="C22" t="s">
+        <v>242</v>
+      </c>
+      <c r="D22">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>332</v>
+      </c>
+      <c r="B23" t="s">
+        <v>328</v>
+      </c>
+      <c r="C23" t="s">
+        <v>248</v>
+      </c>
+      <c r="D23">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>332</v>
+      </c>
+      <c r="B24" t="s">
+        <v>328</v>
+      </c>
+      <c r="C24" t="s">
+        <v>247</v>
+      </c>
+      <c r="D24">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>332</v>
+      </c>
+      <c r="B25" t="s">
+        <v>328</v>
+      </c>
+      <c r="C25" t="s">
+        <v>241</v>
+      </c>
+      <c r="D25">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>332</v>
+      </c>
+      <c r="B26" t="s">
+        <v>328</v>
+      </c>
+      <c r="C26" t="s">
+        <v>329</v>
+      </c>
+      <c r="D26">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>332</v>
+      </c>
+      <c r="B27" t="s">
+        <v>330</v>
+      </c>
+      <c r="C27" t="s">
+        <v>242</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>332</v>
+      </c>
+      <c r="B28" t="s">
+        <v>330</v>
+      </c>
+      <c r="C28" t="s">
+        <v>248</v>
+      </c>
+      <c r="D28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>332</v>
+      </c>
+      <c r="B29" t="s">
+        <v>330</v>
+      </c>
+      <c r="C29" t="s">
+        <v>247</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>332</v>
+      </c>
+      <c r="B30" t="s">
+        <v>330</v>
+      </c>
+      <c r="C30" t="s">
+        <v>241</v>
+      </c>
+      <c r="D30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>332</v>
+      </c>
+      <c r="B31" t="s">
+        <v>330</v>
+      </c>
+      <c r="C31" t="s">
+        <v>329</v>
+      </c>
+      <c r="D31">
+        <v>7.8100000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69EBB41-BAEF-40B9-810D-EC61876EF034}">
   <dimension ref="A1:D31"/>
   <sheetViews>
@@ -2540,10 +3589,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF35CD9C-6566-45D5-AC37-7D32F90348FC}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2756,6 +3805,69 @@
         <v>45.6</v>
       </c>
     </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>384</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="E11" s="30">
+        <v>1</v>
+      </c>
+      <c r="F11" s="30">
+        <f>E11*('Sector data'!$D$35)/1000</f>
+        <v>7.8539816339744819</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="D12" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="E12" s="29">
+        <v>1</v>
+      </c>
+      <c r="F12" s="30">
+        <f>E12*('Sector data'!$D$34)/1000</f>
+        <v>1.5707963267948966</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>384</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="E13" s="30">
+        <v>1</v>
+      </c>
+      <c r="F13" s="30">
+        <f>E13*('Sector data'!$D$34+'Sector data'!$D$35)/1000</f>
+        <v>9.4247779607693793</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2765,10 +3877,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94186171-81A7-4D26-924F-B75D759E6DF5}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2857,7 +3969,7 @@
       <c r="C3" t="s">
         <v>57</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="44">
         <f>2*PI()*G3*H3/360</f>
         <v>1476.5485471872028</v>
       </c>
@@ -2923,7 +4035,7 @@
       <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="44">
         <f>2*PI()*G5*H5/360</f>
         <v>1476.5485471872028</v>
       </c>
@@ -3762,7 +4874,7 @@
       <c r="C31" t="s">
         <v>57</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="44">
         <f>2*PI()*G31*H31/360</f>
         <v>1476.5485471872028</v>
       </c>
@@ -3828,7 +4940,7 @@
       <c r="C33" t="s">
         <v>61</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="44">
         <f>2*PI()*G33*H33/360</f>
         <v>1476.5485471872028</v>
       </c>
@@ -3848,6 +4960,72 @@
         <v>55</v>
       </c>
       <c r="J33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" t="s">
+        <v>395</v>
+      </c>
+      <c r="B34" t="s">
+        <v>391</v>
+      </c>
+      <c r="C34" t="s">
+        <v>393</v>
+      </c>
+      <c r="D34" s="44">
+        <f>2*PI()*G34*H34/360</f>
+        <v>1570.7963267948965</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0.04</v>
+      </c>
+      <c r="G34">
+        <v>1000</v>
+      </c>
+      <c r="H34">
+        <v>90</v>
+      </c>
+      <c r="I34" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>395</v>
+      </c>
+      <c r="B35" t="s">
+        <v>392</v>
+      </c>
+      <c r="C35" t="s">
+        <v>394</v>
+      </c>
+      <c r="D35" s="44">
+        <f>D34*5</f>
+        <v>7853.9816339744821</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>55</v>
+      </c>
+      <c r="J35">
         <v>0</v>
       </c>
     </row>
@@ -3855,15 +5033,18 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D31" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04A54C1-E4DA-444B-8C3A-50F2DC127EAA}">
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7559,6 +8740,340 @@
         <v>0</v>
       </c>
     </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B98" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="C98" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="E98" s="30" t="str">
+        <f>E34</f>
+        <v>Deceleration</v>
+      </c>
+      <c r="F98" s="30">
+        <f t="shared" ref="F98:I98" si="15">F34</f>
+        <v>1</v>
+      </c>
+      <c r="G98">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="H98">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="I98">
+        <f>1000*90/3600</f>
+        <v>25</v>
+      </c>
+      <c r="J98" s="30">
+        <f t="shared" ref="J98:K98" si="16">J34</f>
+        <v>0</v>
+      </c>
+      <c r="K98" s="30">
+        <f>0.1*9.81</f>
+        <v>0.98100000000000009</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B99" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="C99" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="E99" s="30" t="str">
+        <f t="shared" ref="E99:I100" si="17">E35</f>
+        <v>Acceleration</v>
+      </c>
+      <c r="F99" s="30">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="G99" s="30">
+        <v>25</v>
+      </c>
+      <c r="H99">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="I99">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="J99" s="30">
+        <f>0.1*9.81</f>
+        <v>0.98100000000000009</v>
+      </c>
+      <c r="K99" s="30">
+        <f t="shared" ref="J99:K99" si="18">K35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B100" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="C100" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>387</v>
+      </c>
+      <c r="E100" s="30" t="str">
+        <f t="shared" si="17"/>
+        <v>Constant</v>
+      </c>
+      <c r="F100" s="30">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="G100">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="H100">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="I100">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="J100" s="30">
+        <f t="shared" ref="J100:K100" si="19">J36</f>
+        <v>0</v>
+      </c>
+      <c r="K100" s="30">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B101" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="C101" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D101" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="E101" s="30" t="str">
+        <f>E38</f>
+        <v>Constant</v>
+      </c>
+      <c r="F101" s="30">
+        <f t="shared" ref="F101:K101" si="20">F38</f>
+        <v>1</v>
+      </c>
+      <c r="G101">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="H101">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="I101">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="J101" s="30">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K101" s="30">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B102" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C102" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D102" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="E102" s="30" t="str">
+        <f>E38</f>
+        <v>Constant</v>
+      </c>
+      <c r="F102" s="30">
+        <f t="shared" ref="F102:I102" si="21">F38</f>
+        <v>1</v>
+      </c>
+      <c r="G102">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="H102">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="I102">
+        <f>1000*90/3600</f>
+        <v>25</v>
+      </c>
+      <c r="J102" s="30">
+        <f t="shared" ref="J102:K102" si="22">J38</f>
+        <v>0</v>
+      </c>
+      <c r="K102" s="30">
+        <f>0.1*9.81</f>
+        <v>0.98100000000000009</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B103" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C103" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D103" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="E103" s="30" t="str">
+        <f t="shared" ref="E103:I103" si="23">E39</f>
+        <v>Constant</v>
+      </c>
+      <c r="F103" s="30">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="G103" s="30">
+        <v>25</v>
+      </c>
+      <c r="H103">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="I103">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="J103" s="30">
+        <f>0.1*9.81</f>
+        <v>0.98100000000000009</v>
+      </c>
+      <c r="K103" s="30">
+        <f t="shared" ref="K103" si="24">K39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="A104" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B104" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C104" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="D104" s="30" t="s">
+        <v>387</v>
+      </c>
+      <c r="E104" s="30" t="str">
+        <f t="shared" ref="E104:K104" si="25">E40</f>
+        <v>Constant</v>
+      </c>
+      <c r="F104" s="30">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="G104">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="H104">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="I104">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="J104" s="30">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="K104" s="30">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="A105" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B105" s="30" t="s">
+        <v>399</v>
+      </c>
+      <c r="C105" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D105" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="E105" s="30" t="str">
+        <f>E42</f>
+        <v>Constant</v>
+      </c>
+      <c r="F105" s="30">
+        <f t="shared" ref="F105:K105" si="26">F42</f>
+        <v>1</v>
+      </c>
+      <c r="G105">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="H105">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="I105">
+        <f>1000*130/3600</f>
+        <v>36.111111111111114</v>
+      </c>
+      <c r="J105" s="30">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="K105" s="30">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7569,10 +9084,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7F470A-CD1E-4308-B1FA-299B52F2B30A}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7656,7 +9171,7 @@
       <c r="C3" t="s">
         <v>230</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3">
         <f>503+473+461+431</f>
         <v>1868</v>
       </c>
@@ -7703,6 +9218,35 @@
       </c>
       <c r="I4">
         <v>11.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="31" customFormat="1">
+      <c r="A5" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="D5" s="31">
+        <v>1252</v>
+      </c>
+      <c r="E5" s="31">
+        <v>2.7</v>
+      </c>
+      <c r="F5" s="31">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G5" s="31">
+        <v>9.9</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="I5" s="31">
+        <v>10.7</v>
       </c>
     </row>
   </sheetData>
@@ -7716,7 +9260,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7879,8 +9423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3834D1-938D-47C6-97E6-CD34B424831C}">
   <dimension ref="B2:V67"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:G10"/>
+    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -7967,27 +9511,27 @@
         <v>265</v>
       </c>
       <c r="C9" s="15"/>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="35" t="s">
         <v>266</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="34"/>
-      <c r="V9" s="35"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+      <c r="M9" s="36"/>
+      <c r="N9" s="36"/>
+      <c r="O9" s="36"/>
+      <c r="P9" s="36"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="36"/>
+      <c r="V9" s="37"/>
     </row>
     <row r="10" spans="2:22">
       <c r="B10" s="26"/>
@@ -8051,7 +9595,7 @@
       </c>
     </row>
     <row r="11" spans="2:22">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="32" t="s">
         <v>255</v>
       </c>
       <c r="C11" s="17" t="s">
@@ -8116,7 +9660,7 @@
       </c>
     </row>
     <row r="12" spans="2:22">
-      <c r="B12" s="31"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="17" t="s">
         <v>287</v>
       </c>
@@ -8179,7 +9723,7 @@
       </c>
     </row>
     <row r="13" spans="2:22">
-      <c r="B13" s="31"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="17" t="s">
         <v>288</v>
       </c>
@@ -8242,7 +9786,7 @@
       </c>
     </row>
     <row r="14" spans="2:22">
-      <c r="B14" s="31"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="17" t="s">
         <v>289</v>
       </c>
@@ -8305,7 +9849,7 @@
       </c>
     </row>
     <row r="15" spans="2:22">
-      <c r="B15" s="31"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="17" t="s">
         <v>290</v>
       </c>
@@ -8384,7 +9928,7 @@
       </c>
     </row>
     <row r="16" spans="2:22">
-      <c r="B16" s="31"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="17" t="s">
         <v>291</v>
       </c>
@@ -8447,7 +9991,7 @@
       </c>
     </row>
     <row r="17" spans="2:22">
-      <c r="B17" s="32"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="17" t="s">
         <v>292</v>
       </c>
@@ -8533,7 +10077,7 @@
       <c r="V18" s="23"/>
     </row>
     <row r="19" spans="2:22">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="38" t="s">
         <v>293</v>
       </c>
       <c r="C19" s="17" t="s">
@@ -8598,7 +10142,7 @@
       </c>
     </row>
     <row r="20" spans="2:22">
-      <c r="B20" s="37"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="17" t="s">
         <v>287</v>
       </c>
@@ -8661,7 +10205,7 @@
       </c>
     </row>
     <row r="21" spans="2:22">
-      <c r="B21" s="37"/>
+      <c r="B21" s="39"/>
       <c r="C21" s="17" t="s">
         <v>288</v>
       </c>
@@ -8724,7 +10268,7 @@
       </c>
     </row>
     <row r="22" spans="2:22">
-      <c r="B22" s="37"/>
+      <c r="B22" s="39"/>
       <c r="C22" s="17" t="s">
         <v>289</v>
       </c>
@@ -8787,7 +10331,7 @@
       </c>
     </row>
     <row r="23" spans="2:22">
-      <c r="B23" s="37"/>
+      <c r="B23" s="39"/>
       <c r="C23" s="17" t="s">
         <v>290</v>
       </c>
@@ -8866,7 +10410,7 @@
       </c>
     </row>
     <row r="24" spans="2:22">
-      <c r="B24" s="37"/>
+      <c r="B24" s="39"/>
       <c r="C24" s="17" t="s">
         <v>291</v>
       </c>
@@ -8929,7 +10473,7 @@
       </c>
     </row>
     <row r="25" spans="2:22">
-      <c r="B25" s="38"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="17" t="s">
         <v>292</v>
       </c>
@@ -9015,7 +10559,7 @@
       <c r="V26" s="23"/>
     </row>
     <row r="27" spans="2:22">
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="41" t="s">
         <v>294</v>
       </c>
       <c r="C27" s="17" t="s">
@@ -9080,7 +10624,7 @@
       </c>
     </row>
     <row r="28" spans="2:22">
-      <c r="B28" s="40"/>
+      <c r="B28" s="42"/>
       <c r="C28" s="17" t="s">
         <v>287</v>
       </c>
@@ -9143,7 +10687,7 @@
       </c>
     </row>
     <row r="29" spans="2:22">
-      <c r="B29" s="40"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="17" t="s">
         <v>288</v>
       </c>
@@ -9206,7 +10750,7 @@
       </c>
     </row>
     <row r="30" spans="2:22">
-      <c r="B30" s="40"/>
+      <c r="B30" s="42"/>
       <c r="C30" s="17" t="s">
         <v>289</v>
       </c>
@@ -9269,7 +10813,7 @@
       </c>
     </row>
     <row r="31" spans="2:22">
-      <c r="B31" s="40"/>
+      <c r="B31" s="42"/>
       <c r="C31" s="17" t="s">
         <v>290</v>
       </c>
@@ -9348,7 +10892,7 @@
       </c>
     </row>
     <row r="32" spans="2:22">
-      <c r="B32" s="40"/>
+      <c r="B32" s="42"/>
       <c r="C32" s="17" t="s">
         <v>291</v>
       </c>
@@ -9411,7 +10955,7 @@
       </c>
     </row>
     <row r="33" spans="2:22">
-      <c r="B33" s="41"/>
+      <c r="B33" s="43"/>
       <c r="C33" s="17" t="s">
         <v>292</v>
       </c>
@@ -9497,7 +11041,7 @@
       <c r="V34" s="23"/>
     </row>
     <row r="35" spans="2:22">
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="32" t="s">
         <v>238</v>
       </c>
       <c r="C35" s="17" t="s">
@@ -9562,7 +11106,7 @@
       </c>
     </row>
     <row r="36" spans="2:22">
-      <c r="B36" s="31"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="17" t="s">
         <v>287</v>
       </c>
@@ -9625,7 +11169,7 @@
       </c>
     </row>
     <row r="37" spans="2:22">
-      <c r="B37" s="31"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="17" t="s">
         <v>288</v>
       </c>
@@ -9688,7 +11232,7 @@
       </c>
     </row>
     <row r="38" spans="2:22">
-      <c r="B38" s="31"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="17" t="s">
         <v>289</v>
       </c>
@@ -9751,7 +11295,7 @@
       </c>
     </row>
     <row r="39" spans="2:22">
-      <c r="B39" s="31"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="17" t="s">
         <v>290</v>
       </c>
@@ -9830,7 +11374,7 @@
       </c>
     </row>
     <row r="40" spans="2:22">
-      <c r="B40" s="31"/>
+      <c r="B40" s="33"/>
       <c r="C40" s="17" t="s">
         <v>291</v>
       </c>
@@ -9893,7 +11437,7 @@
       </c>
     </row>
     <row r="41" spans="2:22">
-      <c r="B41" s="32"/>
+      <c r="B41" s="34"/>
       <c r="C41" s="17" t="s">
         <v>292</v>
       </c>
@@ -9979,7 +11523,7 @@
       <c r="V42" s="23"/>
     </row>
     <row r="43" spans="2:22">
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="32" t="s">
         <v>244</v>
       </c>
       <c r="C43" s="17" t="s">
@@ -10044,7 +11588,7 @@
       </c>
     </row>
     <row r="44" spans="2:22">
-      <c r="B44" s="31"/>
+      <c r="B44" s="33"/>
       <c r="C44" s="17" t="s">
         <v>287</v>
       </c>
@@ -10107,7 +11651,7 @@
       </c>
     </row>
     <row r="45" spans="2:22">
-      <c r="B45" s="31"/>
+      <c r="B45" s="33"/>
       <c r="C45" s="17" t="s">
         <v>288</v>
       </c>
@@ -10170,7 +11714,7 @@
       </c>
     </row>
     <row r="46" spans="2:22">
-      <c r="B46" s="31"/>
+      <c r="B46" s="33"/>
       <c r="C46" s="17" t="s">
         <v>289</v>
       </c>
@@ -10233,7 +11777,7 @@
       </c>
     </row>
     <row r="47" spans="2:22">
-      <c r="B47" s="31"/>
+      <c r="B47" s="33"/>
       <c r="C47" s="17" t="s">
         <v>290</v>
       </c>
@@ -10312,7 +11856,7 @@
       </c>
     </row>
     <row r="48" spans="2:22">
-      <c r="B48" s="31"/>
+      <c r="B48" s="33"/>
       <c r="C48" s="17" t="s">
         <v>291</v>
       </c>
@@ -10375,7 +11919,7 @@
       </c>
     </row>
     <row r="49" spans="2:22">
-      <c r="B49" s="32"/>
+      <c r="B49" s="34"/>
       <c r="C49" s="17" t="s">
         <v>292</v>
       </c>
@@ -10461,7 +12005,7 @@
       <c r="V50" s="23"/>
     </row>
     <row r="51" spans="2:22">
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="32" t="s">
         <v>249</v>
       </c>
       <c r="C51" s="17" t="s">
@@ -10526,7 +12070,7 @@
       </c>
     </row>
     <row r="52" spans="2:22">
-      <c r="B52" s="31"/>
+      <c r="B52" s="33"/>
       <c r="C52" s="17" t="s">
         <v>287</v>
       </c>
@@ -10589,7 +12133,7 @@
       </c>
     </row>
     <row r="53" spans="2:22">
-      <c r="B53" s="31"/>
+      <c r="B53" s="33"/>
       <c r="C53" s="17" t="s">
         <v>288</v>
       </c>
@@ -10652,7 +12196,7 @@
       </c>
     </row>
     <row r="54" spans="2:22">
-      <c r="B54" s="31"/>
+      <c r="B54" s="33"/>
       <c r="C54" s="17" t="s">
         <v>289</v>
       </c>
@@ -10715,7 +12259,7 @@
       </c>
     </row>
     <row r="55" spans="2:22">
-      <c r="B55" s="31"/>
+      <c r="B55" s="33"/>
       <c r="C55" s="17" t="s">
         <v>290</v>
       </c>
@@ -10794,7 +12338,7 @@
       </c>
     </row>
     <row r="56" spans="2:22">
-      <c r="B56" s="31"/>
+      <c r="B56" s="33"/>
       <c r="C56" s="17" t="s">
         <v>291</v>
       </c>
@@ -10857,7 +12401,7 @@
       </c>
     </row>
     <row r="57" spans="2:22">
-      <c r="B57" s="32"/>
+      <c r="B57" s="34"/>
       <c r="C57" s="17" t="s">
         <v>292</v>
       </c>
@@ -10943,7 +12487,7 @@
       <c r="V58" s="23"/>
     </row>
     <row r="59" spans="2:22">
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="32" t="s">
         <v>252</v>
       </c>
       <c r="C59" s="17" t="s">
@@ -11008,7 +12552,7 @@
       </c>
     </row>
     <row r="60" spans="2:22">
-      <c r="B60" s="31"/>
+      <c r="B60" s="33"/>
       <c r="C60" s="17" t="s">
         <v>287</v>
       </c>
@@ -11071,7 +12615,7 @@
       </c>
     </row>
     <row r="61" spans="2:22">
-      <c r="B61" s="31"/>
+      <c r="B61" s="33"/>
       <c r="C61" s="17" t="s">
         <v>288</v>
       </c>
@@ -11134,7 +12678,7 @@
       </c>
     </row>
     <row r="62" spans="2:22">
-      <c r="B62" s="31"/>
+      <c r="B62" s="33"/>
       <c r="C62" s="17" t="s">
         <v>289</v>
       </c>
@@ -11197,7 +12741,7 @@
       </c>
     </row>
     <row r="63" spans="2:22">
-      <c r="B63" s="31"/>
+      <c r="B63" s="33"/>
       <c r="C63" s="17" t="s">
         <v>290</v>
       </c>
@@ -11276,7 +12820,7 @@
       </c>
     </row>
     <row r="64" spans="2:22">
-      <c r="B64" s="31"/>
+      <c r="B64" s="33"/>
       <c r="C64" s="17" t="s">
         <v>291</v>
       </c>
@@ -11339,7 +12883,7 @@
       </c>
     </row>
     <row r="65" spans="2:22">
-      <c r="B65" s="32"/>
+      <c r="B65" s="34"/>
       <c r="C65" s="17" t="s">
         <v>292</v>
       </c>
@@ -11443,667 +12987,543 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E0172C-DF0F-4DBA-8FF0-B64EC2D7369B}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B7D490-4724-44DB-9756-35EF11163C36}">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" t="s">
+        <v>229</v>
+      </c>
+      <c r="G2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D3" t="s">
+        <v>247</v>
+      </c>
+      <c r="E3" t="s">
+        <v>248</v>
+      </c>
+      <c r="F3" t="s">
+        <v>229</v>
+      </c>
+      <c r="G3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C4" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B5" t="s">
+        <v>340</v>
+      </c>
+      <c r="C5" t="s">
+        <v>357</v>
+      </c>
+      <c r="D5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E5" t="s">
+        <v>248</v>
+      </c>
+      <c r="F5" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B6" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" t="s">
+        <v>358</v>
+      </c>
+      <c r="D6" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F6" t="s">
+        <v>229</v>
+      </c>
+      <c r="G6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B7" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" t="s">
+        <v>359</v>
+      </c>
+      <c r="D7" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" t="s">
+        <v>242</v>
+      </c>
+      <c r="F7" t="s">
+        <v>229</v>
+      </c>
+      <c r="G7" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B8" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" t="s">
+        <v>360</v>
+      </c>
+      <c r="D8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E8" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" t="s">
+        <v>229</v>
+      </c>
+      <c r="G8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C9" t="s">
+        <v>361</v>
+      </c>
+      <c r="D9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" t="s">
+        <v>229</v>
+      </c>
+      <c r="G9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B10" t="s">
+        <v>345</v>
+      </c>
+      <c r="C10" t="s">
+        <v>362</v>
+      </c>
+      <c r="D10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E10" t="s">
+        <v>248</v>
+      </c>
+      <c r="F10" t="s">
+        <v>229</v>
+      </c>
+      <c r="G10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>376</v>
+      </c>
+      <c r="B11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C11" t="s">
+        <v>363</v>
+      </c>
+      <c r="D11" t="s">
+        <v>247</v>
+      </c>
+      <c r="E11" t="s">
+        <v>242</v>
+      </c>
+      <c r="F11" t="s">
+        <v>229</v>
+      </c>
+      <c r="G11" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>377</v>
+      </c>
+      <c r="B12" t="s">
+        <v>347</v>
+      </c>
+      <c r="C12" t="s">
+        <v>364</v>
+      </c>
+      <c r="D12" t="s">
+        <v>247</v>
+      </c>
+      <c r="E12" t="s">
+        <v>242</v>
+      </c>
+      <c r="F12" t="s">
+        <v>229</v>
+      </c>
+      <c r="G12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>378</v>
+      </c>
+      <c r="B13" t="s">
+        <v>348</v>
+      </c>
+      <c r="C13" t="s">
+        <v>365</v>
+      </c>
+      <c r="D13" t="s">
+        <v>242</v>
+      </c>
+      <c r="E13" t="s">
+        <v>248</v>
+      </c>
+      <c r="F13" t="s">
+        <v>229</v>
+      </c>
+      <c r="G13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>379</v>
+      </c>
+      <c r="B14" t="s">
+        <v>349</v>
+      </c>
+      <c r="C14" t="s">
+        <v>366</v>
+      </c>
+      <c r="D14" t="s">
+        <v>247</v>
+      </c>
+      <c r="E14" t="s">
+        <v>242</v>
+      </c>
+      <c r="F14" t="s">
+        <v>229</v>
+      </c>
+      <c r="G14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" t="s">
+        <v>350</v>
+      </c>
+      <c r="C15" t="s">
+        <v>367</v>
+      </c>
+      <c r="D15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E15" t="s">
+        <v>248</v>
+      </c>
+      <c r="F15" t="s">
+        <v>229</v>
+      </c>
+      <c r="G15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>380</v>
+      </c>
+      <c r="B16" t="s">
+        <v>351</v>
+      </c>
+      <c r="C16" t="s">
+        <v>368</v>
+      </c>
+      <c r="D16" t="s">
+        <v>247</v>
+      </c>
+      <c r="E16" t="s">
+        <v>242</v>
+      </c>
+      <c r="F16" t="s">
+        <v>229</v>
+      </c>
+      <c r="G16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33AA0F0-47E1-4AC0-A88E-CD4E07267161}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>295</v>
+        <v>335</v>
       </c>
       <c r="B1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E1" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>300</v>
-      </c>
-      <c r="B2" t="s">
-        <v>301</v>
-      </c>
-      <c r="C2">
-        <v>9.81</v>
-      </c>
-      <c r="D2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>337</v>
+      </c>
+      <c r="B2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C3">
-        <v>0.85</v>
-      </c>
-      <c r="D3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>338</v>
+      </c>
+      <c r="B3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>306</v>
-      </c>
-      <c r="B4" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4">
-        <v>0.13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>339</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>308</v>
-      </c>
-      <c r="B5" t="s">
-        <v>309</v>
-      </c>
-      <c r="C5">
-        <v>0.15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>340</v>
+      </c>
+      <c r="B5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>310</v>
-      </c>
-      <c r="B6" t="s">
-        <v>311</v>
-      </c>
-      <c r="C6">
-        <v>1.2050000000000001</v>
-      </c>
-      <c r="D6" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>341</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>313</v>
-      </c>
-      <c r="B7" t="s">
-        <v>314</v>
-      </c>
-      <c r="C7">
-        <v>1.07</v>
-      </c>
-      <c r="D7" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>342</v>
+      </c>
+      <c r="B7">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B8" t="s">
-        <v>316</v>
-      </c>
-      <c r="C8">
-        <v>1.47</v>
-      </c>
-      <c r="D8" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>343</v>
+      </c>
+      <c r="B8">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>317</v>
-      </c>
-      <c r="B9" t="s">
-        <v>318</v>
-      </c>
-      <c r="C9">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>344</v>
+      </c>
+      <c r="B9">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>319</v>
-      </c>
-      <c r="B10" t="s">
-        <v>318</v>
-      </c>
-      <c r="C10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>345</v>
+      </c>
+      <c r="B10">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>320</v>
-      </c>
-      <c r="B11" t="s">
-        <v>318</v>
-      </c>
-      <c r="C11">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>346</v>
+      </c>
+      <c r="B11">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>321</v>
-      </c>
-      <c r="B12" t="s">
-        <v>318</v>
-      </c>
-      <c r="C12">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>347</v>
+      </c>
+      <c r="B12">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>322</v>
-      </c>
-      <c r="B13" t="s">
-        <v>323</v>
-      </c>
-      <c r="C13">
-        <v>0.68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>324</v>
+        <v>348</v>
+      </c>
+      <c r="B13">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>349</v>
+      </c>
+      <c r="B14">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>350</v>
+      </c>
+      <c r="B15">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>351</v>
+      </c>
+      <c r="B16">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F501E61A-82C5-43C3-BC60-CB8CE2E4C1FF}">
-  <dimension ref="A1:D31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.88671875" customWidth="1"/>
-    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>325</v>
-      </c>
-      <c r="B1" t="s">
-        <v>326</v>
-      </c>
-      <c r="C1" t="s">
-        <v>327</v>
-      </c>
-      <c r="D1" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>229</v>
-      </c>
-      <c r="B2" t="s">
-        <v>328</v>
-      </c>
-      <c r="C2" t="s">
-        <v>242</v>
-      </c>
-      <c r="D2">
-        <v>5.8500000000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B3" t="s">
-        <v>328</v>
-      </c>
-      <c r="C3" t="s">
-        <v>248</v>
-      </c>
-      <c r="D3">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>229</v>
-      </c>
-      <c r="B4" t="s">
-        <v>328</v>
-      </c>
-      <c r="C4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D4">
-        <v>7.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>229</v>
-      </c>
-      <c r="B5" t="s">
-        <v>328</v>
-      </c>
-      <c r="C5" t="s">
-        <v>241</v>
-      </c>
-      <c r="D5">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>229</v>
-      </c>
-      <c r="B6" t="s">
-        <v>328</v>
-      </c>
-      <c r="C6" t="s">
-        <v>329</v>
-      </c>
-      <c r="D6">
-        <v>10.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>229</v>
-      </c>
-      <c r="B7" t="s">
-        <v>330</v>
-      </c>
-      <c r="C7" t="s">
-        <v>242</v>
-      </c>
-      <c r="D7">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>229</v>
-      </c>
-      <c r="B8" t="s">
-        <v>330</v>
-      </c>
-      <c r="C8" t="s">
-        <v>248</v>
-      </c>
-      <c r="D8">
-        <v>7.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>229</v>
-      </c>
-      <c r="B9" t="s">
-        <v>330</v>
-      </c>
-      <c r="C9" t="s">
-        <v>247</v>
-      </c>
-      <c r="D9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>229</v>
-      </c>
-      <c r="B10" t="s">
-        <v>330</v>
-      </c>
-      <c r="C10" t="s">
-        <v>241</v>
-      </c>
-      <c r="D10">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>229</v>
-      </c>
-      <c r="B11" t="s">
-        <v>330</v>
-      </c>
-      <c r="C11" t="s">
-        <v>329</v>
-      </c>
-      <c r="D11">
-        <v>11.66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>331</v>
-      </c>
-      <c r="B12" t="s">
-        <v>328</v>
-      </c>
-      <c r="C12" t="s">
-        <v>242</v>
-      </c>
-      <c r="D12">
-        <v>4.95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>331</v>
-      </c>
-      <c r="B13" t="s">
-        <v>328</v>
-      </c>
-      <c r="C13" t="s">
-        <v>248</v>
-      </c>
-      <c r="D13">
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>331</v>
-      </c>
-      <c r="B14" t="s">
-        <v>328</v>
-      </c>
-      <c r="C14" t="s">
-        <v>247</v>
-      </c>
-      <c r="D14">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>331</v>
-      </c>
-      <c r="B15" t="s">
-        <v>328</v>
-      </c>
-      <c r="C15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D15">
-        <v>8.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>331</v>
-      </c>
-      <c r="B16" t="s">
-        <v>328</v>
-      </c>
-      <c r="C16" t="s">
-        <v>329</v>
-      </c>
-      <c r="D16">
-        <v>9.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>331</v>
-      </c>
-      <c r="B17" t="s">
-        <v>330</v>
-      </c>
-      <c r="C17" t="s">
-        <v>242</v>
-      </c>
-      <c r="D17">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>331</v>
-      </c>
-      <c r="B18" t="s">
-        <v>330</v>
-      </c>
-      <c r="C18" t="s">
-        <v>248</v>
-      </c>
-      <c r="D18">
-        <v>6.7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>331</v>
-      </c>
-      <c r="B19" t="s">
-        <v>330</v>
-      </c>
-      <c r="C19" t="s">
-        <v>247</v>
-      </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>331</v>
-      </c>
-      <c r="B20" t="s">
-        <v>330</v>
-      </c>
-      <c r="C20" t="s">
-        <v>241</v>
-      </c>
-      <c r="D20">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>331</v>
-      </c>
-      <c r="B21" t="s">
-        <v>330</v>
-      </c>
-      <c r="C21" t="s">
-        <v>329</v>
-      </c>
-      <c r="D21">
-        <v>10.01</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>332</v>
-      </c>
-      <c r="B22" t="s">
-        <v>328</v>
-      </c>
-      <c r="C22" t="s">
-        <v>242</v>
-      </c>
-      <c r="D22">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>332</v>
-      </c>
-      <c r="B23" t="s">
-        <v>328</v>
-      </c>
-      <c r="C23" t="s">
-        <v>248</v>
-      </c>
-      <c r="D23">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>332</v>
-      </c>
-      <c r="B24" t="s">
-        <v>328</v>
-      </c>
-      <c r="C24" t="s">
-        <v>247</v>
-      </c>
-      <c r="D24">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>332</v>
-      </c>
-      <c r="B25" t="s">
-        <v>328</v>
-      </c>
-      <c r="C25" t="s">
-        <v>241</v>
-      </c>
-      <c r="D25">
-        <v>6.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>332</v>
-      </c>
-      <c r="B26" t="s">
-        <v>328</v>
-      </c>
-      <c r="C26" t="s">
-        <v>329</v>
-      </c>
-      <c r="D26">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>332</v>
-      </c>
-      <c r="B27" t="s">
-        <v>330</v>
-      </c>
-      <c r="C27" t="s">
-        <v>242</v>
-      </c>
-      <c r="D27">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>332</v>
-      </c>
-      <c r="B28" t="s">
-        <v>330</v>
-      </c>
-      <c r="C28" t="s">
-        <v>248</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>332</v>
-      </c>
-      <c r="B29" t="s">
-        <v>330</v>
-      </c>
-      <c r="C29" t="s">
-        <v>247</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>332</v>
-      </c>
-      <c r="B30" t="s">
-        <v>330</v>
-      </c>
-      <c r="C30" t="s">
-        <v>241</v>
-      </c>
-      <c r="D30">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>332</v>
-      </c>
-      <c r="B31" t="s">
-        <v>330</v>
-      </c>
-      <c r="C31" t="s">
-        <v>329</v>
-      </c>
-      <c r="D31">
-        <v>7.8100000000000005</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0577e6a0-5f74-4659-a81a-c7bdc984432d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12373,22 +13793,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0577e6a0-5f74-4659-a81a-c7bdc984432d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FDE463-4D3F-41EC-839E-DA16C78214B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD6878A0-F687-4E6D-A191-8D8ADCEF84BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="0577e6a0-5f74-4659-a81a-c7bdc984432d"/>
-    <ds:schemaRef ds:uri="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -12414,9 +13834,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD6878A0-F687-4E6D-A191-8D8ADCEF84BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FDE463-4D3F-41EC-839E-DA16C78214B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="0577e6a0-5f74-4659-a81a-c7bdc984432d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Work on calculating emission factors from abrasion coefficients
</commit_message>
<xml_diff>
--- a/data/TWP emission data_IDIADA_v01.xlsx
+++ b/data/TWP emission data_IDIADA_v01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rivmnl.sharepoint.com/sites/LEON-Tyres/Gedeelde documenten/WP3 Microplastics/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rivmnl-my.sharepoint.com/personal/joris_quik_rivm_nl/Documents/Git projects/tyre-friction-abrassion-emission_2024/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1471" documentId="8_{0C357616-BE86-4C54-B640-5799EF490498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86DAB85C-BF67-46AB-B7AF-7C568F21FFD9}"/>
+  <xr:revisionPtr revIDLastSave="1484" documentId="8_{0C357616-BE86-4C54-B640-5799EF490498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37B244EF-BF52-45B0-8683-0D568F2E68BE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1B08EC6D-E4F6-452D-BA0B-C8BBC214CF8F}"/>
   </bookViews>
@@ -313,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="384">
   <si>
     <t>This is a spreadsheet collecting all the data needed to apply the tyre friction abrasion model.</t>
   </si>
@@ -1461,58 +1461,10 @@
     <t>BFGoodrich</t>
   </si>
   <si>
-    <t>Motorway straight</t>
-  </si>
-  <si>
-    <t>Motorway bends</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>MMoWStr1</t>
-  </si>
-  <si>
-    <t>MMoWStr2</t>
-  </si>
-  <si>
-    <t>MMoWStr3</t>
-  </si>
-  <si>
-    <t>MMoWStr4</t>
-  </si>
-  <si>
     <t>Golf 7 Facelift</t>
   </si>
   <si>
     <t>ADAC</t>
-  </si>
-  <si>
-    <t>SIML1</t>
-  </si>
-  <si>
-    <t>SIML2</t>
-  </si>
-  <si>
-    <t>East BendSIML</t>
-  </si>
-  <si>
-    <t>North StraightSIML</t>
-  </si>
-  <si>
-    <t>Oval Outer LaneSIML</t>
-  </si>
-  <si>
-    <t>MotorwaySIML</t>
-  </si>
-  <si>
-    <t>Motorway_SIML</t>
-  </si>
-  <si>
-    <t>Motorway_SIML_straight</t>
-  </si>
-  <si>
-    <t>Motorway_SIML_bend</t>
   </si>
 </sst>
 </file>
@@ -1571,7 +1523,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1611,12 +1563,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1836,7 +1782,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1892,7 +1838,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1929,7 +1875,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda 2" xfId="1" xr:uid="{CFCD8E07-CE35-4F1F-B23D-4B3C1756CB7C}"/>
@@ -3589,16 +3534,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF35CD9C-6566-45D5-AC37-7D32F90348FC}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A11" sqref="A11:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="36.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.44140625" customWidth="1"/>
@@ -3805,69 +3750,6 @@
         <v>45.6</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="30" t="s">
-        <v>382</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>398</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>384</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>395</v>
-      </c>
-      <c r="E11" s="30">
-        <v>1</v>
-      </c>
-      <c r="F11" s="30">
-        <f>E11*('Sector data'!$D$35)/1000</f>
-        <v>7.8539816339744819</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="29" t="s">
-        <v>383</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>399</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>384</v>
-      </c>
-      <c r="D12" s="30" t="s">
-        <v>395</v>
-      </c>
-      <c r="E12" s="29">
-        <v>1</v>
-      </c>
-      <c r="F12" s="30">
-        <f>E12*('Sector data'!$D$34)/1000</f>
-        <v>1.5707963267948966</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="30" t="s">
-        <v>396</v>
-      </c>
-      <c r="B13" s="30" t="s">
-        <v>397</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>384</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>395</v>
-      </c>
-      <c r="E13" s="30">
-        <v>1</v>
-      </c>
-      <c r="F13" s="30">
-        <f>E13*('Sector data'!$D$34+'Sector data'!$D$35)/1000</f>
-        <v>9.4247779607693793</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3877,10 +3759,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94186171-81A7-4D26-924F-B75D759E6DF5}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3969,7 +3851,7 @@
       <c r="C3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="31">
         <f>2*PI()*G3*H3/360</f>
         <v>1476.5485471872028</v>
       </c>
@@ -4035,7 +3917,7 @@
       <c r="C5" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="31">
         <f>2*PI()*G5*H5/360</f>
         <v>1476.5485471872028</v>
       </c>
@@ -4874,7 +4756,7 @@
       <c r="C31" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="44">
+      <c r="D31" s="31">
         <f>2*PI()*G31*H31/360</f>
         <v>1476.5485471872028</v>
       </c>
@@ -4940,7 +4822,7 @@
       <c r="C33" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="44">
+      <c r="D33" s="31">
         <f>2*PI()*G33*H33/360</f>
         <v>1476.5485471872028</v>
       </c>
@@ -4960,72 +4842,6 @@
         <v>55</v>
       </c>
       <c r="J33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" t="s">
-        <v>395</v>
-      </c>
-      <c r="B34" t="s">
-        <v>391</v>
-      </c>
-      <c r="C34" t="s">
-        <v>393</v>
-      </c>
-      <c r="D34" s="44">
-        <f>2*PI()*G34*H34/360</f>
-        <v>1570.7963267948965</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>0.04</v>
-      </c>
-      <c r="G34">
-        <v>1000</v>
-      </c>
-      <c r="H34">
-        <v>90</v>
-      </c>
-      <c r="I34" t="s">
-        <v>55</v>
-      </c>
-      <c r="J34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" t="s">
-        <v>395</v>
-      </c>
-      <c r="B35" t="s">
-        <v>392</v>
-      </c>
-      <c r="C35" t="s">
-        <v>394</v>
-      </c>
-      <c r="D35" s="44">
-        <f>D34*5</f>
-        <v>7853.9816339744821</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
-      <c r="G35">
-        <v>0</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35" t="s">
-        <v>55</v>
-      </c>
-      <c r="J35">
         <v>0</v>
       </c>
     </row>
@@ -5041,10 +4857,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04A54C1-E4DA-444B-8C3A-50F2DC127EAA}">
-  <dimension ref="A1:L105"/>
+  <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A98" sqref="A98:XFD105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8737,340 +8554,6 @@
         <v>0</v>
       </c>
       <c r="K97" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11">
-      <c r="A98" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B98" s="30" t="s">
-        <v>397</v>
-      </c>
-      <c r="C98" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D98" s="30" t="s">
-        <v>385</v>
-      </c>
-      <c r="E98" s="30" t="str">
-        <f>E34</f>
-        <v>Deceleration</v>
-      </c>
-      <c r="F98" s="30">
-        <f t="shared" ref="F98:I98" si="15">F34</f>
-        <v>1</v>
-      </c>
-      <c r="G98">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="H98">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="I98">
-        <f>1000*90/3600</f>
-        <v>25</v>
-      </c>
-      <c r="J98" s="30">
-        <f t="shared" ref="J98:K98" si="16">J34</f>
-        <v>0</v>
-      </c>
-      <c r="K98" s="30">
-        <f>0.1*9.81</f>
-        <v>0.98100000000000009</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11">
-      <c r="A99" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B99" s="30" t="s">
-        <v>397</v>
-      </c>
-      <c r="C99" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D99" s="30" t="s">
-        <v>386</v>
-      </c>
-      <c r="E99" s="30" t="str">
-        <f t="shared" ref="E99:I100" si="17">E35</f>
-        <v>Acceleration</v>
-      </c>
-      <c r="F99" s="30">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="G99" s="30">
-        <v>25</v>
-      </c>
-      <c r="H99">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="I99">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="J99" s="30">
-        <f>0.1*9.81</f>
-        <v>0.98100000000000009</v>
-      </c>
-      <c r="K99" s="30">
-        <f t="shared" ref="J99:K99" si="18">K35</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:11">
-      <c r="A100" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B100" s="30" t="s">
-        <v>397</v>
-      </c>
-      <c r="C100" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D100" s="30" t="s">
-        <v>387</v>
-      </c>
-      <c r="E100" s="30" t="str">
-        <f t="shared" si="17"/>
-        <v>Constant</v>
-      </c>
-      <c r="F100" s="30">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="G100">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="H100">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="I100">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="J100" s="30">
-        <f t="shared" ref="J100:K100" si="19">J36</f>
-        <v>0</v>
-      </c>
-      <c r="K100" s="30">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11">
-      <c r="A101" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B101" s="30" t="s">
-        <v>397</v>
-      </c>
-      <c r="C101" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="D101" s="30" t="s">
-        <v>388</v>
-      </c>
-      <c r="E101" s="30" t="str">
-        <f>E38</f>
-        <v>Constant</v>
-      </c>
-      <c r="F101" s="30">
-        <f t="shared" ref="F101:K101" si="20">F38</f>
-        <v>1</v>
-      </c>
-      <c r="G101">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="H101">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="I101">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="J101" s="30">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="K101" s="30">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11">
-      <c r="A102" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B102" s="30" t="s">
-        <v>398</v>
-      </c>
-      <c r="C102" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D102" s="30" t="s">
-        <v>385</v>
-      </c>
-      <c r="E102" s="30" t="str">
-        <f>E38</f>
-        <v>Constant</v>
-      </c>
-      <c r="F102" s="30">
-        <f t="shared" ref="F102:I102" si="21">F38</f>
-        <v>1</v>
-      </c>
-      <c r="G102">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="H102">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="I102">
-        <f>1000*90/3600</f>
-        <v>25</v>
-      </c>
-      <c r="J102" s="30">
-        <f t="shared" ref="J102:K102" si="22">J38</f>
-        <v>0</v>
-      </c>
-      <c r="K102" s="30">
-        <f>0.1*9.81</f>
-        <v>0.98100000000000009</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11">
-      <c r="A103" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B103" s="30" t="s">
-        <v>398</v>
-      </c>
-      <c r="C103" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D103" s="30" t="s">
-        <v>386</v>
-      </c>
-      <c r="E103" s="30" t="str">
-        <f t="shared" ref="E103:I103" si="23">E39</f>
-        <v>Constant</v>
-      </c>
-      <c r="F103" s="30">
-        <f t="shared" si="23"/>
-        <v>1</v>
-      </c>
-      <c r="G103" s="30">
-        <v>25</v>
-      </c>
-      <c r="H103">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="I103">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="J103" s="30">
-        <f>0.1*9.81</f>
-        <v>0.98100000000000009</v>
-      </c>
-      <c r="K103" s="30">
-        <f t="shared" ref="K103" si="24">K39</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11">
-      <c r="A104" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B104" s="30" t="s">
-        <v>398</v>
-      </c>
-      <c r="C104" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D104" s="30" t="s">
-        <v>387</v>
-      </c>
-      <c r="E104" s="30" t="str">
-        <f t="shared" ref="E104:K104" si="25">E40</f>
-        <v>Constant</v>
-      </c>
-      <c r="F104" s="30">
-        <f t="shared" si="25"/>
-        <v>1</v>
-      </c>
-      <c r="G104">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="H104">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="I104">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="J104" s="30">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="K104" s="30">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11">
-      <c r="A105" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B105" s="30" t="s">
-        <v>399</v>
-      </c>
-      <c r="C105" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="D105" s="30" t="s">
-        <v>388</v>
-      </c>
-      <c r="E105" s="30" t="str">
-        <f>E42</f>
-        <v>Constant</v>
-      </c>
-      <c r="F105" s="30">
-        <f t="shared" ref="F105:K105" si="26">F42</f>
-        <v>1</v>
-      </c>
-      <c r="G105">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="H105">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="I105">
-        <f>1000*130/3600</f>
-        <v>36.111111111111114</v>
-      </c>
-      <c r="J105" s="30">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
-      <c r="K105" s="30">
-        <f t="shared" si="26"/>
         <v>0</v>
       </c>
     </row>
@@ -9220,32 +8703,32 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="31" customFormat="1">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:9" s="30" customFormat="1">
+      <c r="A5" s="30" t="s">
         <v>334</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>389</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>390</v>
-      </c>
-      <c r="D5" s="31">
+      <c r="B5" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="D5" s="30">
         <v>1252</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <v>2.7</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="30">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="30">
         <v>9.9</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="30" t="s">
         <v>229</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="30">
         <v>10.7</v>
       </c>
     </row>
@@ -13518,15 +13001,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FF634CA3F5682C418397C6E4414BCDE3" ma:contentTypeVersion="19" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="dcc84226a5c9737fccd97eea407b26d6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="0577e6a0-5f74-4659-a81a-c7bdc984432d" xmlns:ns3="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="412c1c7c3b81559b33b856787a43d0a8" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -13792,7 +13266,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -13805,15 +13279,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD6878A0-F687-4E6D-A191-8D8ADCEF84BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1A97AFE-C266-46C6-A1B3-B4280223A46E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13833,7 +13308,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7FDE463-4D3F-41EC-839E-DA16C78214B4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="0577e6a0-5f74-4659-a81a-c7bdc984432d"/>
@@ -13849,4 +13324,12 @@
     <ds:schemaRef ds:uri="f5c8fe0e-f8db-4fac-9fd3-e69469f9c90b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD6878A0-F687-4E6D-A191-8D8ADCEF84BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>